<commit_message>
Autentifikacia Admin / Uctovnicka/User
</commit_message>
<xml_diff>
--- a/daco3/Excel/Dochadzka.xlsx
+++ b/daco3/Excel/Dochadzka.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>Meno</t>
   </si>
@@ -379,6 +379,9 @@
     <t>15:58</t>
   </si>
   <si>
+    <t>08:10</t>
+  </si>
+  <si>
     <t>13:34</t>
   </si>
   <si>
@@ -389,6 +392,12 @@
   </si>
   <si>
     <t>11:21</t>
+  </si>
+  <si>
+    <t>06:00</t>
+  </si>
+  <si>
+    <t>06:14</t>
   </si>
   <si>
     <t>Celkovo</t>
@@ -446,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E279"/>
+  <dimension ref="A1:E290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" state="frozen" activePane="bottomLeft"/>
@@ -2734,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E134" s="0" t="s">
         <v>17</v>
@@ -4944,10 +4953,10 @@
         <v>16</v>
       </c>
       <c r="D264" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E264" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="265">
@@ -4961,7 +4970,7 @@
         <v>16</v>
       </c>
       <c r="D265" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E265" s="0" t="s">
         <v>17</v>
@@ -4978,7 +4987,7 @@
         <v>16</v>
       </c>
       <c r="D266" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E266" s="0" t="s">
         <v>17</v>
@@ -4995,7 +5004,7 @@
         <v>16</v>
       </c>
       <c r="D267" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E267" s="0" t="s">
         <v>17</v>
@@ -5003,13 +5012,13 @@
     </row>
     <row r="268">
       <c r="A268" s="0" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="B268" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C268" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D268" s="0" t="s">
         <v>18</v>
@@ -5020,7 +5029,7 @@
     </row>
     <row r="269">
       <c r="A269" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B269" s="0" t="s">
         <v>6</v>
@@ -5029,7 +5038,7 @@
         <v>17</v>
       </c>
       <c r="D269" s="0" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E269" s="0" t="s">
         <v>8</v>
@@ -5037,7 +5046,7 @@
     </row>
     <row r="270">
       <c r="A270" s="0" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B270" s="0" t="s">
         <v>6</v>
@@ -5046,7 +5055,7 @@
         <v>17</v>
       </c>
       <c r="D270" s="0" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E270" s="0" t="s">
         <v>8</v>
@@ -5054,7 +5063,7 @@
     </row>
     <row r="271">
       <c r="A271" s="0" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B271" s="0" t="s">
         <v>6</v>
@@ -5063,7 +5072,7 @@
         <v>17</v>
       </c>
       <c r="D271" s="0" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="E271" s="0" t="s">
         <v>8</v>
@@ -5071,7 +5080,7 @@
     </row>
     <row r="272">
       <c r="A272" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B272" s="0" t="s">
         <v>6</v>
@@ -5080,7 +5089,7 @@
         <v>17</v>
       </c>
       <c r="D272" s="0" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="E272" s="0" t="s">
         <v>8</v>
@@ -5088,7 +5097,7 @@
     </row>
     <row r="273">
       <c r="A273" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B273" s="0" t="s">
         <v>6</v>
@@ -5097,15 +5106,15 @@
         <v>17</v>
       </c>
       <c r="D273" s="0" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="E273" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B274" s="0" t="s">
         <v>6</v>
@@ -5114,7 +5123,7 @@
         <v>17</v>
       </c>
       <c r="D274" s="0" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="E274" s="0" t="s">
         <v>17</v>
@@ -5122,7 +5131,7 @@
     </row>
     <row r="275">
       <c r="A275" s="0" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B275" s="0" t="s">
         <v>6</v>
@@ -5131,7 +5140,7 @@
         <v>17</v>
       </c>
       <c r="D275" s="0" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E275" s="0" t="s">
         <v>17</v>
@@ -5139,7 +5148,7 @@
     </row>
     <row r="276">
       <c r="A276" s="0" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B276" s="0" t="s">
         <v>6</v>
@@ -5148,15 +5157,15 @@
         <v>17</v>
       </c>
       <c r="D276" s="0" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E276" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B277" s="0" t="s">
         <v>6</v>
@@ -5168,12 +5177,12 @@
         <v>42</v>
       </c>
       <c r="E277" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B278" s="0" t="s">
         <v>6</v>
@@ -5182,26 +5191,213 @@
         <v>17</v>
       </c>
       <c r="D278" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E278" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="B279" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C279" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D279" s="0" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="E279" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B280" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C280" s="0">
+        <v>16</v>
+      </c>
+      <c r="D280" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E280" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B281" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C281" s="0">
+        <v>16</v>
+      </c>
+      <c r="D281" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E281" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B282" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C282" s="0">
+        <v>17</v>
+      </c>
+      <c r="D282" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E282" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B283" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C283" s="0">
+        <v>10</v>
+      </c>
+      <c r="D283" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E283" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B284" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C284" s="0">
+        <v>17</v>
+      </c>
+      <c r="D284" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E284" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B285" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C285" s="0">
+        <v>17</v>
+      </c>
+      <c r="D285" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E285" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B286" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C286" s="0">
+        <v>17</v>
+      </c>
+      <c r="D286" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E286" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B287" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C287" s="0">
+        <v>17</v>
+      </c>
+      <c r="D287" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E287" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B288" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C288" s="0">
+        <v>17</v>
+      </c>
+      <c r="D288" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E288" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B289" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C289" s="0">
+        <v>17</v>
+      </c>
+      <c r="D289" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E289" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B290" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C290" s="0">
+        <v>17</v>
+      </c>
+      <c r="D290" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E290" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5235,7 +5431,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
@@ -5246,7 +5442,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
@@ -5257,7 +5453,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4">
@@ -5268,7 +5464,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
@@ -5279,7 +5475,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6">
@@ -5290,7 +5486,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7">
@@ -5301,7 +5497,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8">
@@ -5312,7 +5508,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9">
@@ -5323,7 +5519,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10">
@@ -5334,7 +5530,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11">
@@ -5345,7 +5541,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>